<commit_message>
adding section 8 q 9 final
</commit_message>
<xml_diff>
--- a/HW_2/docs/experiments_graphs.xlsx
+++ b/HW_2/docs/experiments_graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Introduction_to_Artificial_Intelligence_236501\HW_2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100008_{7373C7F8-B06F-43D6-AE55-07FB0F11E1C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100008_{476EA715-2C72-4766-AC3F-6B7DD1C017A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16335" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9344,8 +9344,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4465EF67-D3B7-4512-9520-2F4325CF5F36}">
   <dimension ref="A1:R139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" topLeftCell="E103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N145" sqref="N145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12100,43 +12100,43 @@
         <v>62</v>
       </c>
       <c r="I67" s="7">
-        <f>MAX(I56:I65)</f>
+        <f t="shared" ref="I67:R67" si="0">MAX(I56:I65)</f>
         <v>1937.7142859999999</v>
       </c>
       <c r="J67" s="7">
-        <f>MAX(J56:J65)</f>
+        <f t="shared" si="0"/>
         <v>562</v>
       </c>
       <c r="K67" s="7">
-        <f>MAX(K56:K65)</f>
+        <f t="shared" si="0"/>
         <v>-58.857142860000003</v>
       </c>
       <c r="L67" s="7">
-        <f>MAX(L56:L65)</f>
+        <f t="shared" si="0"/>
         <v>1713.857143</v>
       </c>
       <c r="M67" s="7">
-        <f>MAX(M56:M65)</f>
+        <f t="shared" si="0"/>
         <v>1460.4285709999999</v>
       </c>
       <c r="N67" s="7">
-        <f>MAX(N56:N65)</f>
+        <f t="shared" si="0"/>
         <v>513</v>
       </c>
       <c r="O67" s="7">
-        <f>MAX(O56:O65)</f>
+        <f t="shared" si="0"/>
         <v>1262.142857</v>
       </c>
       <c r="P67" s="7">
-        <f>MAX(P56:P65)</f>
+        <f t="shared" si="0"/>
         <v>1896.7142859999999</v>
       </c>
       <c r="Q67" s="7">
-        <f>MAX(Q56:Q65)</f>
+        <f t="shared" si="0"/>
         <v>2486</v>
       </c>
       <c r="R67" s="7">
-        <f>MAX(R56:R65)</f>
+        <f t="shared" si="0"/>
         <v>348.7142857</v>
       </c>
     </row>

</xml_diff>